<commit_message>
Run all for check
</commit_message>
<xml_diff>
--- a/source_data/cycles_1.xlsx
+++ b/source_data/cycles_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC06B1A-24B3-244E-8510-93CCFC5D6546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B367BC-010F-6A41-ABF4-F1DA1EFF998F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29800" yWindow="6520" windowWidth="35800" windowHeight="16580" activeTab="3" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="29800" yWindow="6520" windowWidth="35800" windowHeight="16580" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -44,10 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="160">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="165">
   <si>
     <t>Epoch</t>
   </si>
@@ -524,6 +521,24 @@
   </si>
   <si>
     <t>otherTimelines</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Main Timeline</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>This is the main timeline for the study design.</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Potential subject identified</t>
   </si>
 </sst>
 </file>
@@ -596,7 +611,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -655,22 +670,31 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1002,98 +1026,98 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B5" t="s">
         <v>127</v>
-      </c>
-      <c r="B5" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" t="s">
         <v>129</v>
-      </c>
-      <c r="B6" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="22" t="s">
         <v>146</v>
-      </c>
-      <c r="B7" s="22" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="C9" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="D9" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="E9" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="F9" s="20" t="s">
         <v>135</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="G9" s="20" t="s">
         <v>136</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="H9" s="20" t="s">
         <v>137</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="C10" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="D10" s="18" t="s">
         <v>141</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>142</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1103,33 +1127,33 @@
         <v>40179</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="C11" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>141</v>
-      </c>
       <c r="D11" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G11" s="21">
         <v>40544</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1153,42 +1177,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>48</v>
-      </c>
       <c r="F1" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1200,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B66121-AE3C-4E48-906B-C59A3DAEA708}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1211,91 +1235,91 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+        <v>52</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
+        <v>55</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+        <v>56</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+        <v>57</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>151</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+        <v>58</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+        <v>157</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+        <v>158</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
@@ -1307,41 +1331,41 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>60</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>63</v>
-      </c>
       <c r="C11" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1380,8 +1404,8 @@
   </sheetPr>
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1399,18 +1423,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="26" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>3</v>
       </c>
       <c r="F1" s="26"/>
       <c r="G1" s="26"/>
@@ -1421,17 +1447,21 @@
       <c r="L1" s="26"/>
       <c r="M1" s="26"/>
       <c r="N1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>162</v>
+      </c>
       <c r="C2" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="26">
         <v>1</v>
@@ -1446,390 +1476,393 @@
       </c>
       <c r="J2" s="26"/>
       <c r="K2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
+      <c r="A3" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>164</v>
+      </c>
       <c r="C3" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H3" s="26"/>
       <c r="I3" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J3" s="26"/>
       <c r="K3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="26" t="s">
         <v>23</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>24</v>
       </c>
       <c r="F4" s="26"/>
       <c r="G4" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H4" s="26"/>
       <c r="I4" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="26"/>
       <c r="K4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="28"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="27"/>
+      <c r="K5" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="6" t="s">
+      <c r="M5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="28"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="N5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="1" t="s">
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="28"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>22</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="E12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="13">
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E1:M1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A1:B8"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="E3:F3"/>
@@ -1861,72 +1894,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>70</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="14" t="s">
         <v>73</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>76</v>
-      </c>
-      <c r="D3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
         <v>72</v>
       </c>
-      <c r="C4" t="s">
-        <v>73</v>
-      </c>
       <c r="D4" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
         <v>75</v>
       </c>
-      <c r="C5" t="s">
-        <v>76</v>
-      </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1953,70 +1986,70 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="C1" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="D1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="E1" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2">
         <v>100</v>
       </c>
       <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" t="s">
         <v>87</v>
-      </c>
-      <c r="E2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" t="s">
         <v>90</v>
-      </c>
-      <c r="E3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4">
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" t="s">
         <v>93</v>
-      </c>
-      <c r="E4" t="s">
-        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2040,45 +2073,45 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2106,54 +2139,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="G1" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="H1" s="17" t="s">
         <v>109</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
         <v>111</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>112</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>113</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>114</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>115</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>116</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>117</v>
-      </c>
-      <c r="H2" t="s">
-        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2176,18 +2209,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" t="s">
         <v>152</v>
-      </c>
-      <c r="B1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix cycles study details
</commit_message>
<xml_diff>
--- a/source_data/cycles_1.xlsx
+++ b/source_data/cycles_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/timepoints/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B367BC-010F-6A41-ABF4-F1DA1EFF998F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EEF66E-5146-924A-88E8-E6B4622BBEEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29800" yWindow="6520" windowWidth="35800" windowHeight="16580" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="29800" yWindow="6520" windowWidth="35800" windowHeight="16580" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -415,9 +415,6 @@
     <t>OBJ1</t>
   </si>
   <si>
-    <t>Simple Test 1</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -427,15 +424,9 @@
     <t>studyAcronym</t>
   </si>
   <si>
-    <t>SIMPLE</t>
-  </si>
-  <si>
     <t>studyRationale</t>
   </si>
   <si>
-    <t>A simple test</t>
-  </si>
-  <si>
     <t>briefTitle</t>
   </si>
   <si>
@@ -539,6 +530,15 @@
   </si>
   <si>
     <t>Potential subject identified</t>
+  </si>
+  <si>
+    <t>Cycles Test 1</t>
+  </si>
+  <si>
+    <t>CYCLES 1</t>
+  </si>
+  <si>
+    <t>A cycles test</t>
   </si>
 </sst>
 </file>
@@ -669,6 +669,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -683,18 +695,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1012,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F975A6-8C40-A94B-B707-4567CE298AC4}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1029,7 +1029,7 @@
         <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1037,7 +1037,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1045,7 +1045,7 @@
         <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1058,66 +1058,66 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="E9" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="F9" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="G9" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="H9" s="20" t="s">
         <v>134</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>135</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="H9" s="20" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>138</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>141</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
@@ -1127,33 +1127,33 @@
         <v>40179</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C11" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="18" t="s">
         <v>140</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>143</v>
       </c>
       <c r="E11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G11" s="21">
         <v>40544</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +1206,7 @@
         <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>51</v>
@@ -1224,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B66121-AE3C-4E48-906B-C59A3DAEA708}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1237,89 +1237,89 @@
       <c r="A1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
+      <c r="B3" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>148</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
+      <c r="B4" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="B5" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="B6" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+        <v>154</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+        <v>155</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="9"/>
@@ -1423,11 +1423,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="B1" s="28" t="s">
-        <v>160</v>
+      <c r="A1" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>157</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>0</v>
@@ -1435,27 +1435,27 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
       <c r="N1" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>162</v>
+      <c r="A2" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>159</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>3</v>
@@ -1463,18 +1463,18 @@
       <c r="D2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="26">
+      <c r="E2" s="30">
         <v>1</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26">
+      <c r="F2" s="30"/>
+      <c r="G2" s="30">
         <v>2</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26">
+      <c r="H2" s="30"/>
+      <c r="I2" s="30">
         <v>3</v>
       </c>
-      <c r="J2" s="26"/>
+      <c r="J2" s="30"/>
       <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1489,11 +1489,11 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>164</v>
+      <c r="A3" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>161</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>30</v>
@@ -1501,18 +1501,18 @@
       <c r="D3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26" t="s">
+      <c r="F3" s="30"/>
+      <c r="G3" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26" t="s">
+      <c r="H3" s="30"/>
+      <c r="I3" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="26"/>
+      <c r="J3" s="30"/>
       <c r="K3" s="1" t="s">
         <v>28</v>
       </c>
@@ -1527,26 +1527,26 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26" t="s">
+      <c r="F4" s="30"/>
+      <c r="G4" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26" t="s">
+      <c r="H4" s="30"/>
+      <c r="I4" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="26"/>
+      <c r="J4" s="30"/>
       <c r="K4" s="1" t="s">
         <v>23</v>
       </c>
@@ -1561,28 +1561,28 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="27"/>
+      <c r="E5" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="31"/>
       <c r="K5" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>24</v>
@@ -1595,8 +1595,8 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
@@ -1635,8 +1635,8 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
@@ -1675,8 +1675,8 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
@@ -1859,6 +1859,9 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E1:M1"/>
     <mergeCell ref="G2:H2"/>
@@ -1869,9 +1872,6 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="57" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -2209,18 +2209,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>